<commit_message>
Raise an error on missing xlsx template row types (#391)
* Raise an error on missing xlsx template row types

* Resolve black version conflict in precommit hook

* Address PR comments

* Set service column width
</commit_message>
<xml_diff>
--- a/tests/data/date_examples.xlsx
+++ b/tests/data/date_examples.xlsx
@@ -1,63 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/schemas/tests/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="6740" windowWidth="26960" windowHeight="15380" tabRatio="500" activeTab="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5760" yWindow="6740" windowWidth="26960" windowHeight="15380" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="150000" fullCalcOnLoad="1" concurrentCalc="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>slashes</t>
-  </si>
-  <si>
-    <t>slashes-txt</t>
-  </si>
-  <si>
-    <t>1/12/1998</t>
-  </si>
-  <si>
-    <t>time-bad</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -76,22 +47,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -357,29 +322,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="A1" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>slashes</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n">
         <v>35807</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>slashes-txt</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>1/12/1998</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -388,25 +363,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>time-bad</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n">
         <v>35807</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
+    <row r="2">
+      <c r="B2" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>